<commit_message>
in merge with spaceclaim
</commit_message>
<xml_diff>
--- a/tests/Модель_пористости.xlsx
+++ b/tests/Модель_пористости.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\QForm_practice\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C92EB5-DC73-49FB-A102-C837AC9E3988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A19FE0-6E05-4926-84A7-0D59EE8AD333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B21538D7-078E-4EB9-B170-17AEBD1D8C35}"/>
   </bookViews>
@@ -42,12 +42,6 @@
     <t>геометрия</t>
   </si>
   <si>
-    <t>куб</t>
-  </si>
-  <si>
-    <t>сфера</t>
-  </si>
-  <si>
     <t>пористость, %</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>Средние напряжения (статистика), МПа</t>
   </si>
   <si>
-    <t>эллипс</t>
-  </si>
-  <si>
     <t>Доп. параметр 1</t>
   </si>
   <si>
@@ -73,6 +64,15 @@
   </si>
   <si>
     <t>Доп. параметр 3</t>
+  </si>
+  <si>
+    <t>cube</t>
+  </si>
+  <si>
+    <t>sphere</t>
+  </si>
+  <si>
+    <t>ellipse</t>
   </si>
 </sst>
 </file>
@@ -435,8 +435,8 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D260" sqref="D260"/>
+      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J218" sqref="J218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -466,30 +466,30 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
       <c r="L1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>0.01</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0.01</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>0.01</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0.01</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0.01</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>0.01</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0.01</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0.01</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.01</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>0.01</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0.01</v>
@@ -720,7 +720,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0.01</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>0.01</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>0.01</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>0.01</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>0.01</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>0.1</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>0.1</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>0.1</v>
@@ -888,7 +888,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>0.1</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B22">
         <v>0.1</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>0.1</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B24">
         <v>0.1</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B25">
         <v>0.1</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B26">
         <v>0.1</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B27">
         <v>0.1</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B28">
         <v>0.1</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B29">
         <v>0.1</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B30">
         <v>0.1</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B31">
         <v>0.1</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B32">
         <v>0.1</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B33">
         <v>0.1</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1266,7 +1266,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1350,7 +1350,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B50">
         <v>5</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B51">
         <v>5</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B52">
         <v>5</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B53">
         <v>5</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B54">
         <v>5</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B55">
         <v>5</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B57">
         <v>5</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B58">
         <v>5</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B59">
         <v>5</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B60">
         <v>5</v>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B61">
         <v>5</v>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B62">
         <v>5</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B63">
         <v>5</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B64">
         <v>5</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B66">
         <v>10</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B67">
         <v>10</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B68">
         <v>10</v>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B69">
         <v>10</v>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B70">
         <v>10</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B71">
         <v>10</v>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B72">
         <v>10</v>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B73">
         <v>10</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B74">
         <v>10</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B75">
         <v>10</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B76">
         <v>10</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B77">
         <v>10</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B78">
         <v>10</v>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B79">
         <v>10</v>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B80">
         <v>10</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B81">
         <v>10</v>
@@ -2169,7 +2169,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B82">
         <v>20</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B83">
         <v>20</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B84">
         <v>20</v>
@@ -2232,7 +2232,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B85">
         <v>20</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B86">
         <v>20</v>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B87">
         <v>20</v>
@@ -2295,7 +2295,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B88">
         <v>20</v>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B89">
         <v>20</v>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B90">
         <v>20</v>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B91">
         <v>20</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B92">
         <v>20</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B93">
         <v>20</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B94">
         <v>20</v>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B95">
         <v>20</v>
@@ -2463,7 +2463,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B96">
         <v>20</v>
@@ -2484,7 +2484,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B97">
         <v>20</v>
@@ -2505,7 +2505,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B98">
         <v>25</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B99">
         <v>25</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B100">
         <v>25</v>
@@ -2568,7 +2568,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B101">
         <v>25</v>
@@ -2589,7 +2589,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B102">
         <v>25</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B103">
         <v>25</v>
@@ -2631,7 +2631,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B104">
         <v>25</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B105">
         <v>25</v>
@@ -2673,7 +2673,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B106">
         <v>25</v>
@@ -2694,7 +2694,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B107">
         <v>25</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B108">
         <v>25</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B109">
         <v>25</v>
@@ -2757,7 +2757,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B110">
         <v>25</v>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B111">
         <v>25</v>
@@ -2799,7 +2799,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B112">
         <v>25</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B113">
         <v>25</v>
@@ -2841,7 +2841,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B114">
         <v>0.01</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B115">
         <v>0.01</v>
@@ -2883,7 +2883,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B116">
         <v>0.01</v>
@@ -2904,7 +2904,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B117">
         <v>0.01</v>
@@ -2925,7 +2925,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B118">
         <v>0.01</v>
@@ -2946,7 +2946,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B119">
         <v>0.01</v>
@@ -2967,7 +2967,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B120">
         <v>0.01</v>
@@ -2988,7 +2988,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B121">
         <v>0.01</v>
@@ -3009,7 +3009,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B122">
         <v>0.01</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B123">
         <v>0.01</v>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B124">
         <v>0.01</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B125">
         <v>0.01</v>
@@ -3093,7 +3093,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B126">
         <v>0.01</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B127">
         <v>0.01</v>
@@ -3135,7 +3135,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B128">
         <v>0.01</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B129">
         <v>0.01</v>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B130">
         <v>0.1</v>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B131">
         <v>0.1</v>
@@ -3219,7 +3219,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B132">
         <v>0.1</v>
@@ -3240,7 +3240,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B133">
         <v>0.1</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B134">
         <v>0.1</v>
@@ -3282,7 +3282,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B135">
         <v>0.1</v>
@@ -3303,7 +3303,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B136">
         <v>0.1</v>
@@ -3324,7 +3324,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B137">
         <v>0.1</v>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B138">
         <v>0.1</v>
@@ -3366,7 +3366,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B139">
         <v>0.1</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B140">
         <v>0.1</v>
@@ -3408,7 +3408,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B141">
         <v>0.1</v>
@@ -3429,7 +3429,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B142">
         <v>0.1</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B143">
         <v>0.1</v>
@@ -3471,7 +3471,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B144">
         <v>0.1</v>
@@ -3492,7 +3492,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B145">
         <v>0.1</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -3534,7 +3534,7 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -3555,7 +3555,7 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -3576,7 +3576,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B149">
         <v>1</v>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B150">
         <v>1</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -3639,7 +3639,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B152">
         <v>1</v>
@@ -3660,7 +3660,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B153">
         <v>1</v>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B154">
         <v>1</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B155">
         <v>1</v>
@@ -3723,7 +3723,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -3744,7 +3744,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -3765,7 +3765,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B158">
         <v>1</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -3807,7 +3807,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -3828,7 +3828,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -3849,7 +3849,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B162">
         <v>5</v>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B163">
         <v>5</v>
@@ -3891,7 +3891,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B164">
         <v>5</v>
@@ -3912,7 +3912,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B165">
         <v>5</v>
@@ -3933,7 +3933,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B166">
         <v>5</v>
@@ -3954,7 +3954,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B167">
         <v>5</v>
@@ -3975,7 +3975,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B168">
         <v>5</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B169">
         <v>5</v>
@@ -4017,7 +4017,7 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B170">
         <v>5</v>
@@ -4038,7 +4038,7 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B171">
         <v>5</v>
@@ -4059,7 +4059,7 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B172">
         <v>5</v>
@@ -4080,7 +4080,7 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B173">
         <v>5</v>
@@ -4101,7 +4101,7 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B174">
         <v>5</v>
@@ -4122,7 +4122,7 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B175">
         <v>5</v>
@@ -4143,7 +4143,7 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B176">
         <v>5</v>
@@ -4164,7 +4164,7 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B177">
         <v>5</v>
@@ -4185,7 +4185,7 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B178">
         <v>10</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B179">
         <v>10</v>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B180">
         <v>10</v>
@@ -4248,7 +4248,7 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B181">
         <v>10</v>
@@ -4269,7 +4269,7 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B182">
         <v>10</v>
@@ -4290,7 +4290,7 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B183">
         <v>10</v>
@@ -4311,7 +4311,7 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B184">
         <v>10</v>
@@ -4332,7 +4332,7 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B185">
         <v>10</v>
@@ -4353,7 +4353,7 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B186">
         <v>10</v>
@@ -4374,7 +4374,7 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B187">
         <v>10</v>
@@ -4395,7 +4395,7 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B188">
         <v>10</v>
@@ -4416,7 +4416,7 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B189">
         <v>10</v>
@@ -4437,7 +4437,7 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B190">
         <v>10</v>
@@ -4458,7 +4458,7 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B191">
         <v>10</v>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B192">
         <v>10</v>
@@ -4500,7 +4500,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B193">
         <v>10</v>
@@ -4521,7 +4521,7 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B194">
         <v>20</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B195">
         <v>20</v>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B196">
         <v>20</v>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B197">
         <v>20</v>
@@ -4605,7 +4605,7 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B198">
         <v>20</v>
@@ -4626,7 +4626,7 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B199">
         <v>20</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B200">
         <v>20</v>
@@ -4668,7 +4668,7 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B201">
         <v>20</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B202">
         <v>20</v>
@@ -4710,7 +4710,7 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B203">
         <v>20</v>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B204">
         <v>20</v>
@@ -4752,7 +4752,7 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B205">
         <v>20</v>
@@ -4773,7 +4773,7 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B206">
         <v>20</v>
@@ -4794,7 +4794,7 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B207">
         <v>20</v>
@@ -4815,7 +4815,7 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B208">
         <v>20</v>
@@ -4836,7 +4836,7 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B209">
         <v>20</v>
@@ -4857,7 +4857,7 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B210">
         <v>25</v>
@@ -4878,7 +4878,7 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B211">
         <v>25</v>
@@ -4899,7 +4899,7 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B212">
         <v>25</v>
@@ -4920,7 +4920,7 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B213">
         <v>25</v>
@@ -4941,7 +4941,7 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B214">
         <v>25</v>
@@ -4962,7 +4962,7 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B215">
         <v>25</v>
@@ -4983,7 +4983,7 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B216">
         <v>25</v>
@@ -5004,7 +5004,7 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B217">
         <v>25</v>
@@ -5025,7 +5025,7 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B218">
         <v>25</v>
@@ -5046,7 +5046,7 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B219">
         <v>25</v>
@@ -5067,7 +5067,7 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B220">
         <v>25</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B221">
         <v>25</v>
@@ -5109,7 +5109,7 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B222">
         <v>25</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B223">
         <v>25</v>
@@ -5151,7 +5151,7 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B224">
         <v>25</v>
@@ -5172,7 +5172,7 @@
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B225">
         <v>25</v>
@@ -5193,7 +5193,7 @@
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B226">
         <v>0.01</v>
@@ -5223,7 +5223,7 @@
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B227">
         <v>0.01</v>
@@ -5253,7 +5253,7 @@
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B228">
         <v>0.01</v>
@@ -5283,7 +5283,7 @@
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B229">
         <v>0.01</v>
@@ -5313,7 +5313,7 @@
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B230">
         <v>0.01</v>
@@ -5343,7 +5343,7 @@
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B231">
         <v>0.01</v>
@@ -5373,7 +5373,7 @@
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B232">
         <v>0.01</v>
@@ -5403,7 +5403,7 @@
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B233">
         <v>0.01</v>
@@ -5433,7 +5433,7 @@
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B234">
         <v>0.01</v>
@@ -5463,7 +5463,7 @@
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B235">
         <v>0.01</v>
@@ -5493,7 +5493,7 @@
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B236">
         <v>0.01</v>
@@ -5523,7 +5523,7 @@
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B237">
         <v>0.01</v>
@@ -5553,7 +5553,7 @@
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B238">
         <v>0.01</v>
@@ -5583,7 +5583,7 @@
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B239">
         <v>0.01</v>
@@ -5613,7 +5613,7 @@
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B240">
         <v>0.01</v>
@@ -5643,7 +5643,7 @@
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B241">
         <v>0.01</v>
@@ -5673,7 +5673,7 @@
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B242">
         <v>0.1</v>
@@ -5703,7 +5703,7 @@
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B243">
         <v>0.1</v>
@@ -5733,7 +5733,7 @@
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B244">
         <v>0.1</v>
@@ -5763,7 +5763,7 @@
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B245">
         <v>0.1</v>
@@ -5793,7 +5793,7 @@
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B246">
         <v>0.1</v>
@@ -5823,7 +5823,7 @@
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B247">
         <v>0.1</v>
@@ -5853,7 +5853,7 @@
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B248">
         <v>0.1</v>
@@ -5883,7 +5883,7 @@
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B249">
         <v>0.1</v>
@@ -5913,7 +5913,7 @@
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B250">
         <v>0.1</v>
@@ -5943,7 +5943,7 @@
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B251">
         <v>0.1</v>
@@ -5973,7 +5973,7 @@
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B252">
         <v>0.1</v>
@@ -6003,7 +6003,7 @@
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B253">
         <v>0.1</v>
@@ -6033,7 +6033,7 @@
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B254">
         <v>0.1</v>
@@ -6063,7 +6063,7 @@
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B255">
         <v>0.1</v>
@@ -6093,7 +6093,7 @@
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B256">
         <v>0.1</v>
@@ -6123,7 +6123,7 @@
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B257">
         <v>0.1</v>
@@ -6153,7 +6153,7 @@
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B258">
         <v>1</v>
@@ -6183,7 +6183,7 @@
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B259">
         <v>1</v>
@@ -6213,7 +6213,7 @@
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B260">
         <v>1</v>
@@ -6243,7 +6243,7 @@
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B261">
         <v>1</v>
@@ -6273,7 +6273,7 @@
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B262">
         <v>1</v>
@@ -6303,7 +6303,7 @@
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B263">
         <v>1</v>
@@ -6333,7 +6333,7 @@
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B264">
         <v>1</v>
@@ -6363,7 +6363,7 @@
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B265">
         <v>1</v>
@@ -6393,7 +6393,7 @@
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B266">
         <v>1</v>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B267">
         <v>1</v>
@@ -6453,7 +6453,7 @@
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B268">
         <v>1</v>
@@ -6483,7 +6483,7 @@
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B269">
         <v>1</v>
@@ -6513,7 +6513,7 @@
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B270">
         <v>1</v>
@@ -6543,7 +6543,7 @@
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B271">
         <v>1</v>
@@ -6573,7 +6573,7 @@
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B272">
         <v>1</v>
@@ -6603,7 +6603,7 @@
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B273">
         <v>1</v>
@@ -6633,7 +6633,7 @@
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B274">
         <v>5</v>
@@ -6663,7 +6663,7 @@
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B275">
         <v>5</v>
@@ -6693,7 +6693,7 @@
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B276">
         <v>5</v>
@@ -6723,7 +6723,7 @@
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B277">
         <v>5</v>
@@ -6753,7 +6753,7 @@
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B278">
         <v>5</v>
@@ -6783,7 +6783,7 @@
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B279">
         <v>5</v>
@@ -6813,7 +6813,7 @@
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B280">
         <v>5</v>
@@ -6843,7 +6843,7 @@
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B281">
         <v>5</v>
@@ -6873,7 +6873,7 @@
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B282">
         <v>5</v>
@@ -6903,7 +6903,7 @@
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B283">
         <v>5</v>
@@ -6933,7 +6933,7 @@
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B284">
         <v>5</v>
@@ -6963,7 +6963,7 @@
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B285">
         <v>5</v>
@@ -6993,7 +6993,7 @@
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B286">
         <v>5</v>
@@ -7023,7 +7023,7 @@
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B287">
         <v>5</v>
@@ -7053,7 +7053,7 @@
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B288">
         <v>5</v>
@@ -7083,7 +7083,7 @@
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B289">
         <v>5</v>
@@ -7113,7 +7113,7 @@
     </row>
     <row r="290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B290">
         <v>0.01</v>
@@ -7143,7 +7143,7 @@
     </row>
     <row r="291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B291">
         <v>0.01</v>
@@ -7173,7 +7173,7 @@
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B292">
         <v>0.01</v>
@@ -7203,7 +7203,7 @@
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B293">
         <v>0.01</v>
@@ -7233,7 +7233,7 @@
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B294">
         <v>0.01</v>
@@ -7263,7 +7263,7 @@
     </row>
     <row r="295" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B295">
         <v>0.01</v>
@@ -7293,7 +7293,7 @@
     </row>
     <row r="296" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B296">
         <v>0.01</v>
@@ -7323,7 +7323,7 @@
     </row>
     <row r="297" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B297">
         <v>0.01</v>
@@ -7353,7 +7353,7 @@
     </row>
     <row r="298" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B298">
         <v>0.01</v>
@@ -7383,7 +7383,7 @@
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B299">
         <v>0.01</v>
@@ -7413,7 +7413,7 @@
     </row>
     <row r="300" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B300">
         <v>0.01</v>
@@ -7443,7 +7443,7 @@
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B301">
         <v>0.01</v>
@@ -7473,7 +7473,7 @@
     </row>
     <row r="302" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B302">
         <v>0.01</v>
@@ -7503,7 +7503,7 @@
     </row>
     <row r="303" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B303">
         <v>0.01</v>
@@ -7533,7 +7533,7 @@
     </row>
     <row r="304" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B304">
         <v>0.01</v>
@@ -7563,7 +7563,7 @@
     </row>
     <row r="305" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B305">
         <v>0.01</v>
@@ -7593,7 +7593,7 @@
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B306">
         <v>0.1</v>
@@ -7623,7 +7623,7 @@
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B307">
         <v>0.1</v>
@@ -7653,7 +7653,7 @@
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B308">
         <v>0.1</v>
@@ -7683,7 +7683,7 @@
     </row>
     <row r="309" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B309">
         <v>0.1</v>
@@ -7713,7 +7713,7 @@
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B310">
         <v>0.1</v>
@@ -7743,7 +7743,7 @@
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B311">
         <v>0.1</v>
@@ -7773,7 +7773,7 @@
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B312">
         <v>0.1</v>
@@ -7803,7 +7803,7 @@
     </row>
     <row r="313" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B313">
         <v>0.1</v>
@@ -7833,7 +7833,7 @@
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B314">
         <v>0.1</v>
@@ -7863,7 +7863,7 @@
     </row>
     <row r="315" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B315">
         <v>0.1</v>
@@ -7893,7 +7893,7 @@
     </row>
     <row r="316" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B316">
         <v>0.1</v>
@@ -7923,7 +7923,7 @@
     </row>
     <row r="317" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B317">
         <v>0.1</v>
@@ -7953,7 +7953,7 @@
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B318">
         <v>0.1</v>
@@ -7983,7 +7983,7 @@
     </row>
     <row r="319" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B319">
         <v>0.1</v>
@@ -8013,7 +8013,7 @@
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B320">
         <v>0.1</v>
@@ -8043,7 +8043,7 @@
     </row>
     <row r="321" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B321">
         <v>0.1</v>
@@ -8073,7 +8073,7 @@
     </row>
     <row r="322" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B322">
         <v>1</v>
@@ -8103,7 +8103,7 @@
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B323">
         <v>1</v>
@@ -8133,7 +8133,7 @@
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B324">
         <v>1</v>
@@ -8163,7 +8163,7 @@
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B325">
         <v>1</v>
@@ -8193,7 +8193,7 @@
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B326">
         <v>1</v>
@@ -8223,7 +8223,7 @@
     </row>
     <row r="327" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B327">
         <v>1</v>
@@ -8253,7 +8253,7 @@
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B328">
         <v>1</v>
@@ -8283,7 +8283,7 @@
     </row>
     <row r="329" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B329">
         <v>1</v>
@@ -8313,7 +8313,7 @@
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B330">
         <v>1</v>
@@ -8343,7 +8343,7 @@
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B331">
         <v>1</v>
@@ -8373,7 +8373,7 @@
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B332">
         <v>1</v>
@@ -8403,7 +8403,7 @@
     </row>
     <row r="333" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B333">
         <v>1</v>
@@ -8433,7 +8433,7 @@
     </row>
     <row r="334" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B334">
         <v>1</v>
@@ -8463,7 +8463,7 @@
     </row>
     <row r="335" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B335">
         <v>1</v>
@@ -8493,7 +8493,7 @@
     </row>
     <row r="336" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B336">
         <v>1</v>
@@ -8523,7 +8523,7 @@
     </row>
     <row r="337" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B337">
         <v>1</v>
@@ -8553,7 +8553,7 @@
     </row>
     <row r="338" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B338">
         <v>5</v>
@@ -8583,7 +8583,7 @@
     </row>
     <row r="339" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B339">
         <v>5</v>
@@ -8613,7 +8613,7 @@
     </row>
     <row r="340" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B340">
         <v>5</v>
@@ -8643,7 +8643,7 @@
     </row>
     <row r="341" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B341">
         <v>5</v>
@@ -8673,7 +8673,7 @@
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B342">
         <v>5</v>
@@ -8703,7 +8703,7 @@
     </row>
     <row r="343" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B343">
         <v>5</v>
@@ -8733,7 +8733,7 @@
     </row>
     <row r="344" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B344">
         <v>5</v>
@@ -8763,7 +8763,7 @@
     </row>
     <row r="345" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B345">
         <v>5</v>
@@ -8793,7 +8793,7 @@
     </row>
     <row r="346" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B346">
         <v>5</v>
@@ -8823,7 +8823,7 @@
     </row>
     <row r="347" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B347">
         <v>5</v>
@@ -8853,7 +8853,7 @@
     </row>
     <row r="348" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B348">
         <v>5</v>
@@ -8883,7 +8883,7 @@
     </row>
     <row r="349" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B349">
         <v>5</v>
@@ -8913,7 +8913,7 @@
     </row>
     <row r="350" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B350">
         <v>5</v>
@@ -8943,7 +8943,7 @@
     </row>
     <row r="351" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B351">
         <v>5</v>
@@ -8973,7 +8973,7 @@
     </row>
     <row r="352" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B352">
         <v>5</v>
@@ -9003,7 +9003,7 @@
     </row>
     <row r="353" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B353">
         <v>5</v>
@@ -9033,7 +9033,7 @@
     </row>
     <row r="354" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B354">
         <v>0.01</v>
@@ -9063,7 +9063,7 @@
     </row>
     <row r="355" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B355">
         <v>0.01</v>
@@ -9093,7 +9093,7 @@
     </row>
     <row r="356" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B356">
         <v>0.01</v>
@@ -9123,7 +9123,7 @@
     </row>
     <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B357">
         <v>0.01</v>
@@ -9153,7 +9153,7 @@
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B358">
         <v>0.01</v>
@@ -9183,7 +9183,7 @@
     </row>
     <row r="359" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B359">
         <v>0.01</v>
@@ -9213,7 +9213,7 @@
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B360">
         <v>0.01</v>
@@ -9243,7 +9243,7 @@
     </row>
     <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B361">
         <v>0.01</v>
@@ -9273,7 +9273,7 @@
     </row>
     <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B362">
         <v>0.01</v>
@@ -9303,7 +9303,7 @@
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B363">
         <v>0.01</v>
@@ -9333,7 +9333,7 @@
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B364">
         <v>0.01</v>
@@ -9363,7 +9363,7 @@
     </row>
     <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B365">
         <v>0.01</v>
@@ -9393,7 +9393,7 @@
     </row>
     <row r="366" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B366">
         <v>0.01</v>
@@ -9423,7 +9423,7 @@
     </row>
     <row r="367" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B367">
         <v>0.01</v>
@@ -9453,7 +9453,7 @@
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B368">
         <v>0.01</v>
@@ -9483,7 +9483,7 @@
     </row>
     <row r="369" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B369">
         <v>0.01</v>
@@ -9513,7 +9513,7 @@
     </row>
     <row r="370" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B370">
         <v>0.1</v>
@@ -9543,7 +9543,7 @@
     </row>
     <row r="371" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B371">
         <v>0.1</v>
@@ -9573,7 +9573,7 @@
     </row>
     <row r="372" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B372">
         <v>0.1</v>
@@ -9603,7 +9603,7 @@
     </row>
     <row r="373" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B373">
         <v>0.1</v>
@@ -9633,7 +9633,7 @@
     </row>
     <row r="374" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B374">
         <v>0.1</v>
@@ -9663,7 +9663,7 @@
     </row>
     <row r="375" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B375">
         <v>0.1</v>
@@ -9693,7 +9693,7 @@
     </row>
     <row r="376" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B376">
         <v>0.1</v>
@@ -9723,7 +9723,7 @@
     </row>
     <row r="377" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B377">
         <v>0.1</v>
@@ -9753,7 +9753,7 @@
     </row>
     <row r="378" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B378">
         <v>0.1</v>
@@ -9783,7 +9783,7 @@
     </row>
     <row r="379" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B379">
         <v>0.1</v>
@@ -9813,7 +9813,7 @@
     </row>
     <row r="380" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B380">
         <v>0.1</v>
@@ -9843,7 +9843,7 @@
     </row>
     <row r="381" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B381">
         <v>0.1</v>
@@ -9873,7 +9873,7 @@
     </row>
     <row r="382" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B382">
         <v>0.1</v>
@@ -9903,7 +9903,7 @@
     </row>
     <row r="383" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B383">
         <v>0.1</v>
@@ -9933,7 +9933,7 @@
     </row>
     <row r="384" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B384">
         <v>0.1</v>
@@ -9963,7 +9963,7 @@
     </row>
     <row r="385" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B385">
         <v>0.1</v>
@@ -9993,7 +9993,7 @@
     </row>
     <row r="386" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B386">
         <v>1</v>
@@ -10023,7 +10023,7 @@
     </row>
     <row r="387" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B387">
         <v>1</v>
@@ -10053,7 +10053,7 @@
     </row>
     <row r="388" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B388">
         <v>1</v>
@@ -10083,7 +10083,7 @@
     </row>
     <row r="389" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B389">
         <v>1</v>
@@ -10113,7 +10113,7 @@
     </row>
     <row r="390" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B390">
         <v>1</v>
@@ -10143,7 +10143,7 @@
     </row>
     <row r="391" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B391">
         <v>1</v>
@@ -10173,7 +10173,7 @@
     </row>
     <row r="392" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B392">
         <v>1</v>
@@ -10203,7 +10203,7 @@
     </row>
     <row r="393" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B393">
         <v>1</v>
@@ -10233,7 +10233,7 @@
     </row>
     <row r="394" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B394">
         <v>1</v>
@@ -10263,7 +10263,7 @@
     </row>
     <row r="395" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B395">
         <v>1</v>
@@ -10293,7 +10293,7 @@
     </row>
     <row r="396" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B396">
         <v>1</v>
@@ -10323,7 +10323,7 @@
     </row>
     <row r="397" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B397">
         <v>1</v>
@@ -10353,7 +10353,7 @@
     </row>
     <row r="398" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B398">
         <v>1</v>
@@ -10383,7 +10383,7 @@
     </row>
     <row r="399" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B399">
         <v>1</v>
@@ -10413,7 +10413,7 @@
     </row>
     <row r="400" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B400">
         <v>1</v>
@@ -10443,7 +10443,7 @@
     </row>
     <row r="401" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B401">
         <v>1</v>
@@ -10473,7 +10473,7 @@
     </row>
     <row r="402" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B402">
         <v>5</v>
@@ -10503,7 +10503,7 @@
     </row>
     <row r="403" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B403">
         <v>5</v>
@@ -10533,7 +10533,7 @@
     </row>
     <row r="404" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B404">
         <v>5</v>
@@ -10563,7 +10563,7 @@
     </row>
     <row r="405" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B405">
         <v>5</v>
@@ -10593,7 +10593,7 @@
     </row>
     <row r="406" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B406">
         <v>5</v>
@@ -10623,7 +10623,7 @@
     </row>
     <row r="407" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B407">
         <v>5</v>
@@ -10653,7 +10653,7 @@
     </row>
     <row r="408" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B408">
         <v>5</v>
@@ -10683,7 +10683,7 @@
     </row>
     <row r="409" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B409">
         <v>5</v>
@@ -10713,7 +10713,7 @@
     </row>
     <row r="410" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B410">
         <v>5</v>
@@ -10743,7 +10743,7 @@
     </row>
     <row r="411" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B411">
         <v>5</v>
@@ -10773,7 +10773,7 @@
     </row>
     <row r="412" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B412">
         <v>5</v>
@@ -10803,7 +10803,7 @@
     </row>
     <row r="413" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B413">
         <v>5</v>
@@ -10833,7 +10833,7 @@
     </row>
     <row r="414" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B414">
         <v>5</v>
@@ -10863,7 +10863,7 @@
     </row>
     <row r="415" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B415">
         <v>5</v>
@@ -10893,7 +10893,7 @@
     </row>
     <row r="416" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B416">
         <v>5</v>
@@ -10923,7 +10923,7 @@
     </row>
     <row r="417" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B417">
         <v>5</v>

</xml_diff>